<commit_message>
them Top3 mon ban chay
</commit_message>
<xml_diff>
--- a/GUI_QuanLyCafe/bin/Debug/Image/NhanVien/ThongKe.xlsx
+++ b/GUI_QuanLyCafe/bin/Debug/Image/NhanVien/ThongKe.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DB98ACF-4E25-421C-A55B-167D8A11E98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E08FB075-D08F-491B-B2C0-FBCCFD31C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2355" windowWidth="20730" windowHeight="11835" xr2:uid="{BA1176C1-A7B8-4233-A13B-7E5D17457A1B}"/>
+    <workbookView xWindow="2595" yWindow="2355" windowWidth="20730" windowHeight="11835" xr2:uid="{5E638A52-C8C3-4792-AA51-8AF6CB40A5C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Doanh thu" sheetId="1" r:id="rId1"/>
@@ -27,27 +27,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>DOANH THU THÁNG 12</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+  <si>
+    <t>DOANH THU 28/11/2021 00:00:00 ĐẾN 10/12/2021 23:59:59</t>
   </si>
   <si>
     <t>Thời gian</t>
   </si>
   <si>
-    <t>Tổng tiền</t>
-  </si>
-  <si>
-    <t>Wed 29/12/2021</t>
-  </si>
-  <si>
-    <t>Tue 21/12/2021</t>
-  </si>
-  <si>
-    <t>Wed 01/12/2021</t>
-  </si>
-  <si>
-    <t>Tổng doanh thu : 376,200 VNĐ</t>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Tống</t>
+  </si>
+  <si>
+    <t>Ca tối</t>
+  </si>
+  <si>
+    <t>Nguyễn Tăng Thanh Phương</t>
+  </si>
+  <si>
+    <t>Trác Phương Kiệt</t>
+  </si>
+  <si>
+    <t>29/11/2021 16:08:52</t>
+  </si>
+  <si>
+    <t>29/11/2021 02:54:54</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu : 510,400 VNĐ</t>
   </si>
 </sst>
 </file>
@@ -92,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -102,67 +117,112 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -194,28 +254,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -534,59 +606,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB3160D-FD0B-4374-A54C-51470A788EFB}">
-  <dimension ref="B2:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AF1FDA-0F6A-4290-90D4-1C0FA739B8DE}">
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6328125" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6">
-        <v>150700</v>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="7">
+        <v>44481.740243055552</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="8">
+        <v>323400</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6">
-        <v>193600</v>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="7">
+        <v>44208.854814814818</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8">
+        <v>31900</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8">
-        <v>31900</v>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8">
+        <v>63800</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C9" s="9" t="s">
-        <v>6</v>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12">
+        <v>91300</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>